<commit_message>
Version 2.0 OK, delete version 1.0 file and remove track xlsx, keep file about Version 3.0
</commit_message>
<xml_diff>
--- a/data/cartoon_data.xlsx
+++ b/data/cartoon_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="121">
   <si>
     <t>grade_score</t>
   </si>
@@ -82,9 +82,6 @@
     <t>brp98b7hisskggo</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>pfrcxv33zwkjwk1</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
   </si>
   <si>
     <t>mafnc5yt0np7zml</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>y6p70mcuf0btfq3</t>
@@ -820,8 +814,8 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -874,7 +868,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="n">
         <v>9.187150000000001</v>
@@ -888,8 +882,8 @@
       <c r="E3" t="n">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -942,7 +936,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="n">
         <v>7.99602</v>
@@ -956,8 +950,8 @@
       <c r="E4" t="n">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -1010,7 +1004,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="n">
         <v>5.68274</v>
@@ -1024,8 +1018,8 @@
       <c r="E5" t="n">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -1078,7 +1072,7 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>5.88153</v>
@@ -1092,8 +1086,8 @@
       <c r="E6" t="n">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
-        <v>22</v>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -1146,7 +1140,7 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="n">
         <v>8.39176</v>
@@ -1160,8 +1154,8 @@
       <c r="E7" t="n">
         <v>6</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -1214,7 +1208,7 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="n">
         <v>5.7432</v>
@@ -1228,8 +1222,8 @@
       <c r="E8" t="n">
         <v>49</v>
       </c>
-      <c r="F8" t="s">
-        <v>22</v>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -1282,7 +1276,7 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="n">
         <v>8.376899999999999</v>
@@ -1296,8 +1290,8 @@
       <c r="E9" t="n">
         <v>10</v>
       </c>
-      <c r="F9" t="s">
-        <v>22</v>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -1350,7 +1344,7 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="n">
         <v>5.12916</v>
@@ -1364,8 +1358,8 @@
       <c r="E10" t="n">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>22</v>
+      <c r="F10" t="n">
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -1418,7 +1412,7 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="n">
         <v>7.1036</v>
@@ -1432,8 +1426,8 @@
       <c r="E11" t="n">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
-        <v>22</v>
+      <c r="F11" t="n">
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -1486,7 +1480,7 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="n">
         <v>9.563269999999999</v>
@@ -1500,8 +1494,8 @@
       <c r="E12" t="n">
         <v>5</v>
       </c>
-      <c r="F12" t="s">
-        <v>22</v>
+      <c r="F12" t="n">
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>1</v>
@@ -1554,7 +1548,7 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="n">
         <v>7.83471</v>
@@ -1568,8 +1562,8 @@
       <c r="E13" t="n">
         <v>12</v>
       </c>
-      <c r="F13" t="s">
-        <v>22</v>
+      <c r="F13" t="n">
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -1622,7 +1616,7 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="n">
         <v>6.98969</v>
@@ -1636,8 +1630,8 @@
       <c r="E14" t="n">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
-        <v>22</v>
+      <c r="F14" t="n">
+        <v>0</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -1690,7 +1684,7 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="n">
         <v>8.419079999999999</v>
@@ -1704,8 +1698,8 @@
       <c r="E15" t="n">
         <v>12</v>
       </c>
-      <c r="F15" t="s">
-        <v>22</v>
+      <c r="F15" t="n">
+        <v>0</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -1758,7 +1752,7 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="n">
         <v>9.711169999999999</v>
@@ -1772,8 +1766,8 @@
       <c r="E16" t="n">
         <v>14</v>
       </c>
-      <c r="F16" t="s">
-        <v>22</v>
+      <c r="F16" t="n">
+        <v>0</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
@@ -1826,7 +1820,7 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="n">
         <v>6.74433</v>
@@ -1840,8 +1834,8 @@
       <c r="E17" t="n">
         <v>3</v>
       </c>
-      <c r="F17" t="s">
-        <v>22</v>
+      <c r="F17" t="n">
+        <v>0</v>
       </c>
       <c r="G17" t="n">
         <v>1</v>
@@ -1894,7 +1888,7 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="n">
         <v>4.97482</v>
@@ -1908,8 +1902,8 @@
       <c r="E18" t="n">
         <v>2</v>
       </c>
-      <c r="F18" t="s">
-        <v>22</v>
+      <c r="F18" t="n">
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
@@ -1962,7 +1956,7 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" t="n">
         <v>5.25105</v>
@@ -1976,8 +1970,8 @@
       <c r="E19" t="n">
         <v>48</v>
       </c>
-      <c r="F19" t="s">
-        <v>22</v>
+      <c r="F19" t="n">
+        <v>0</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -2030,7 +2024,7 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="n">
         <v>7.71596</v>
@@ -2044,8 +2038,8 @@
       <c r="E20" t="n">
         <v>15</v>
       </c>
-      <c r="F20" t="s">
-        <v>22</v>
+      <c r="F20" t="n">
+        <v>0</v>
       </c>
       <c r="G20" t="n">
         <v>1</v>
@@ -2098,7 +2092,7 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="n">
         <v>9.42905</v>
@@ -2112,8 +2106,8 @@
       <c r="E21" t="n">
         <v>21</v>
       </c>
-      <c r="F21" t="s">
-        <v>22</v>
+      <c r="F21" t="n">
+        <v>0</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>
@@ -2166,7 +2160,7 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="n">
         <v>7.92984</v>
@@ -2180,8 +2174,8 @@
       <c r="E22" t="n">
         <v>21</v>
       </c>
-      <c r="F22" t="s">
-        <v>22</v>
+      <c r="F22" t="n">
+        <v>0</v>
       </c>
       <c r="G22" t="n">
         <v>1</v>
@@ -2234,7 +2228,7 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" t="n">
         <v>8.90629</v>
@@ -2248,8 +2242,8 @@
       <c r="E23" t="n">
         <v>22</v>
       </c>
-      <c r="F23" t="s">
-        <v>22</v>
+      <c r="F23" t="n">
+        <v>0</v>
       </c>
       <c r="G23" t="n">
         <v>1</v>
@@ -2302,7 +2296,7 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="n">
         <v>6.88613</v>
@@ -2316,8 +2310,8 @@
       <c r="E24" t="n">
         <v>23</v>
       </c>
-      <c r="F24" t="s">
-        <v>22</v>
+      <c r="F24" t="n">
+        <v>0</v>
       </c>
       <c r="G24" t="n">
         <v>1</v>
@@ -2370,7 +2364,7 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="n">
         <v>8.184189999999999</v>
@@ -2384,8 +2378,8 @@
       <c r="E25" t="n">
         <v>11</v>
       </c>
-      <c r="F25" t="s">
-        <v>22</v>
+      <c r="F25" t="n">
+        <v>0</v>
       </c>
       <c r="G25" t="n">
         <v>1</v>
@@ -2438,7 +2432,7 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" t="n">
         <v>8.90274</v>
@@ -2452,8 +2446,8 @@
       <c r="E26" t="n">
         <v>23</v>
       </c>
-      <c r="F26" t="s">
-        <v>22</v>
+      <c r="F26" t="n">
+        <v>0</v>
       </c>
       <c r="G26" t="n">
         <v>1</v>
@@ -2506,7 +2500,7 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="n">
         <v>6.13028</v>
@@ -2520,8 +2514,8 @@
       <c r="E27" t="n">
         <v>1</v>
       </c>
-      <c r="F27" t="s">
-        <v>22</v>
+      <c r="F27" t="n">
+        <v>0</v>
       </c>
       <c r="G27" t="n">
         <v>1</v>
@@ -2574,7 +2568,7 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" t="n">
         <v>6.58861</v>
@@ -2588,8 +2582,8 @@
       <c r="E28" t="n">
         <v>3</v>
       </c>
-      <c r="F28" t="s">
-        <v>22</v>
+      <c r="F28" t="n">
+        <v>0</v>
       </c>
       <c r="G28" t="n">
         <v>1</v>
@@ -2642,7 +2636,7 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" t="n">
         <v>4.62657</v>
@@ -2656,8 +2650,8 @@
       <c r="E29" t="n">
         <v>12</v>
       </c>
-      <c r="F29" t="s">
-        <v>22</v>
+      <c r="F29" t="n">
+        <v>0</v>
       </c>
       <c r="G29" t="n">
         <v>1</v>
@@ -2710,7 +2704,7 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" t="n">
         <v>5.91038</v>
@@ -2724,8 +2718,8 @@
       <c r="E30" t="n">
         <v>1</v>
       </c>
-      <c r="F30" t="s">
-        <v>22</v>
+      <c r="F30" t="n">
+        <v>0</v>
       </c>
       <c r="G30" t="n">
         <v>1</v>
@@ -2778,7 +2772,7 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" t="n">
         <v>5.56676</v>
@@ -2792,8 +2786,8 @@
       <c r="E31" t="n">
         <v>25</v>
       </c>
-      <c r="F31" t="s">
-        <v>22</v>
+      <c r="F31" t="n">
+        <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>1</v>
@@ -2846,7 +2840,7 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" t="n">
         <v>7.246</v>
@@ -2860,8 +2854,8 @@
       <c r="E32" t="n">
         <v>9</v>
       </c>
-      <c r="F32" t="s">
-        <v>22</v>
+      <c r="F32" t="n">
+        <v>0</v>
       </c>
       <c r="G32" t="n">
         <v>1</v>
@@ -2914,7 +2908,7 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" t="n">
         <v>5.18042</v>
@@ -2928,8 +2922,8 @@
       <c r="E33" t="n">
         <v>4</v>
       </c>
-      <c r="F33" t="s">
-        <v>22</v>
+      <c r="F33" t="n">
+        <v>0</v>
       </c>
       <c r="G33" t="n">
         <v>1</v>
@@ -2982,7 +2976,7 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" t="n">
         <v>6.02189</v>
@@ -2996,8 +2990,8 @@
       <c r="E34" t="n">
         <v>7</v>
       </c>
-      <c r="F34" t="s">
-        <v>22</v>
+      <c r="F34" t="n">
+        <v>0</v>
       </c>
       <c r="G34" t="n">
         <v>1</v>
@@ -3050,7 +3044,7 @@
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" t="n">
         <v>4.44869</v>
@@ -3064,8 +3058,8 @@
       <c r="E35" t="n">
         <v>54</v>
       </c>
-      <c r="F35" t="s">
-        <v>22</v>
+      <c r="F35" t="n">
+        <v>0</v>
       </c>
       <c r="G35" t="n">
         <v>1</v>
@@ -3118,7 +3112,7 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" t="n">
         <v>9.300000000000001</v>
@@ -3132,8 +3126,8 @@
       <c r="E36" t="n">
         <v>20</v>
       </c>
-      <c r="F36" t="s">
-        <v>22</v>
+      <c r="F36" t="n">
+        <v>0</v>
       </c>
       <c r="G36" t="n">
         <v>1</v>
@@ -3186,7 +3180,7 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" t="n">
         <v>8.28257</v>
@@ -3200,8 +3194,8 @@
       <c r="E37" t="n">
         <v>2</v>
       </c>
-      <c r="F37" t="s">
-        <v>22</v>
+      <c r="F37" t="n">
+        <v>0</v>
       </c>
       <c r="G37" t="n">
         <v>1</v>
@@ -3254,7 +3248,7 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" t="n">
         <v>9.34661</v>
@@ -3268,8 +3262,8 @@
       <c r="E38" t="n">
         <v>7</v>
       </c>
-      <c r="F38" t="s">
-        <v>22</v>
+      <c r="F38" t="n">
+        <v>0</v>
       </c>
       <c r="G38" t="n">
         <v>1</v>
@@ -3322,7 +3316,7 @@
     </row>
     <row r="39" spans="1:22">
       <c r="A39" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" t="n">
         <v>6.22965</v>
@@ -3336,8 +3330,8 @@
       <c r="E39" t="n">
         <v>2</v>
       </c>
-      <c r="F39" t="s">
-        <v>22</v>
+      <c r="F39" t="n">
+        <v>0</v>
       </c>
       <c r="G39" t="n">
         <v>1</v>
@@ -3390,7 +3384,7 @@
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" t="n">
         <v>5.94825</v>
@@ -3404,8 +3398,8 @@
       <c r="E40" t="n">
         <v>10</v>
       </c>
-      <c r="F40" t="s">
-        <v>22</v>
+      <c r="F40" t="n">
+        <v>0</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
@@ -3458,20 +3452,22 @@
     </row>
     <row r="41" spans="1:22">
       <c r="A41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" t="n">
         <v>9.628410000000001</v>
       </c>
-      <c r="C41" t="s"/>
+      <c r="C41" t="n">
+        <v>2015</v>
+      </c>
       <c r="D41" t="n">
         <v>272</v>
       </c>
       <c r="E41" t="n">
         <v>4</v>
       </c>
-      <c r="F41" t="s">
-        <v>22</v>
+      <c r="F41" t="n">
+        <v>0</v>
       </c>
       <c r="G41" t="n">
         <v>1</v>
@@ -3524,7 +3520,7 @@
     </row>
     <row r="42" spans="1:22">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" t="n">
         <v>9.49437</v>
@@ -3538,8 +3534,8 @@
       <c r="E42" t="n">
         <v>5</v>
       </c>
-      <c r="F42" t="s">
-        <v>22</v>
+      <c r="F42" t="n">
+        <v>0</v>
       </c>
       <c r="G42" t="n">
         <v>1</v>
@@ -3592,7 +3588,7 @@
     </row>
     <row r="43" spans="1:22">
       <c r="A43" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" t="n">
         <v>5.96477</v>
@@ -3606,8 +3602,8 @@
       <c r="E43" t="n">
         <v>9</v>
       </c>
-      <c r="F43" t="s">
-        <v>22</v>
+      <c r="F43" t="n">
+        <v>0</v>
       </c>
       <c r="G43" t="n">
         <v>1</v>
@@ -3660,7 +3656,7 @@
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" t="n">
         <v>5.32642</v>
@@ -3674,8 +3670,8 @@
       <c r="E44" t="n">
         <v>23</v>
       </c>
-      <c r="F44" t="s">
-        <v>22</v>
+      <c r="F44" t="n">
+        <v>0</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
@@ -3728,7 +3724,7 @@
     </row>
     <row r="45" spans="1:22">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" t="n">
         <v>5.30272</v>
@@ -3742,8 +3738,8 @@
       <c r="E45" t="n">
         <v>23</v>
       </c>
-      <c r="F45" t="s">
-        <v>22</v>
+      <c r="F45" t="n">
+        <v>0</v>
       </c>
       <c r="G45" t="n">
         <v>1</v>
@@ -3796,7 +3792,7 @@
     </row>
     <row r="46" spans="1:22">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46" t="n">
         <v>5.13741</v>
@@ -3810,8 +3806,8 @@
       <c r="E46" t="n">
         <v>23</v>
       </c>
-      <c r="F46" t="s">
-        <v>22</v>
+      <c r="F46" t="n">
+        <v>0</v>
       </c>
       <c r="G46" t="n">
         <v>1</v>
@@ -3864,7 +3860,7 @@
     </row>
     <row r="47" spans="1:22">
       <c r="A47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" t="n">
         <v>8.139279999999999</v>
@@ -3878,8 +3874,8 @@
       <c r="E47" t="n">
         <v>2</v>
       </c>
-      <c r="F47" t="s">
-        <v>22</v>
+      <c r="F47" t="n">
+        <v>0</v>
       </c>
       <c r="G47" t="n">
         <v>1</v>
@@ -3932,7 +3928,7 @@
     </row>
     <row r="48" spans="1:22">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" t="n">
         <v>5.66433</v>
@@ -3946,8 +3942,8 @@
       <c r="E48" t="n">
         <v>12</v>
       </c>
-      <c r="F48" t="s">
-        <v>22</v>
+      <c r="F48" t="n">
+        <v>0</v>
       </c>
       <c r="G48" t="n">
         <v>1</v>
@@ -4000,7 +3996,7 @@
     </row>
     <row r="49" spans="1:22">
       <c r="A49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49" t="n">
         <v>5.9139</v>
@@ -4014,8 +4010,8 @@
       <c r="E49" t="n">
         <v>4</v>
       </c>
-      <c r="F49" t="s">
-        <v>22</v>
+      <c r="F49" t="n">
+        <v>0</v>
       </c>
       <c r="G49" t="n">
         <v>1</v>
@@ -4068,7 +4064,7 @@
     </row>
     <row r="50" spans="1:22">
       <c r="A50" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50" t="n">
         <v>6.3675</v>
@@ -4082,8 +4078,8 @@
       <c r="E50" t="n">
         <v>16</v>
       </c>
-      <c r="F50" t="s">
-        <v>22</v>
+      <c r="F50" t="n">
+        <v>0</v>
       </c>
       <c r="G50" t="n">
         <v>1</v>
@@ -4136,7 +4132,7 @@
     </row>
     <row r="51" spans="1:22">
       <c r="A51" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" t="n">
         <v>8.984859999999999</v>
@@ -4150,8 +4146,8 @@
       <c r="E51" t="n">
         <v>2</v>
       </c>
-      <c r="F51" t="s">
-        <v>22</v>
+      <c r="F51" t="n">
+        <v>0</v>
       </c>
       <c r="G51" t="n">
         <v>1</v>
@@ -4204,7 +4200,7 @@
     </row>
     <row r="52" spans="1:22">
       <c r="A52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52" t="n">
         <v>5.64543</v>
@@ -4218,8 +4214,8 @@
       <c r="E52" t="n">
         <v>19</v>
       </c>
-      <c r="F52" t="s">
-        <v>73</v>
+      <c r="F52" t="n">
+        <v>1</v>
       </c>
       <c r="G52" t="n">
         <v>1</v>
@@ -4272,7 +4268,7 @@
     </row>
     <row r="53" spans="1:22">
       <c r="A53" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B53" t="n">
         <v>5.07768</v>
@@ -4286,8 +4282,8 @@
       <c r="E53" t="n">
         <v>0</v>
       </c>
-      <c r="F53" t="s">
-        <v>22</v>
+      <c r="F53" t="n">
+        <v>0</v>
       </c>
       <c r="G53" t="n">
         <v>1</v>
@@ -4340,7 +4336,7 @@
     </row>
     <row r="54" spans="1:22">
       <c r="A54" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B54" t="n">
         <v>9.23002</v>
@@ -4354,8 +4350,8 @@
       <c r="E54" t="n">
         <v>1</v>
       </c>
-      <c r="F54" t="s">
-        <v>22</v>
+      <c r="F54" t="n">
+        <v>0</v>
       </c>
       <c r="G54" t="n">
         <v>1</v>
@@ -4408,7 +4404,7 @@
     </row>
     <row r="55" spans="1:22">
       <c r="A55" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B55" t="n">
         <v>8.96574</v>
@@ -4422,8 +4418,8 @@
       <c r="E55" t="n">
         <v>6</v>
       </c>
-      <c r="F55" t="s">
-        <v>22</v>
+      <c r="F55" t="n">
+        <v>0</v>
       </c>
       <c r="G55" t="n">
         <v>1</v>
@@ -4476,7 +4472,7 @@
     </row>
     <row r="56" spans="1:22">
       <c r="A56" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B56" t="n">
         <v>4.40523</v>
@@ -4490,8 +4486,8 @@
       <c r="E56" t="n">
         <v>1</v>
       </c>
-      <c r="F56" t="s">
-        <v>22</v>
+      <c r="F56" t="n">
+        <v>0</v>
       </c>
       <c r="G56" t="n">
         <v>1</v>
@@ -4544,7 +4540,7 @@
     </row>
     <row r="57" spans="1:22">
       <c r="A57" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B57" t="n">
         <v>5.6606</v>
@@ -4558,8 +4554,8 @@
       <c r="E57" t="n">
         <v>0</v>
       </c>
-      <c r="F57" t="s">
-        <v>22</v>
+      <c r="F57" t="n">
+        <v>0</v>
       </c>
       <c r="G57" t="n">
         <v>1</v>
@@ -4612,7 +4608,7 @@
     </row>
     <row r="58" spans="1:22">
       <c r="A58" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B58" t="n">
         <v>4.72432</v>
@@ -4626,8 +4622,8 @@
       <c r="E58" t="n">
         <v>0</v>
       </c>
-      <c r="F58" t="s">
-        <v>22</v>
+      <c r="F58" t="n">
+        <v>0</v>
       </c>
       <c r="G58" t="n">
         <v>1</v>
@@ -4680,20 +4676,22 @@
     </row>
     <row r="59" spans="1:22">
       <c r="A59" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B59" t="n">
         <v>8.23563</v>
       </c>
-      <c r="C59" t="s"/>
+      <c r="C59" t="n">
+        <v>2015</v>
+      </c>
       <c r="D59" t="n">
         <v>70</v>
       </c>
       <c r="E59" t="n">
         <v>1</v>
       </c>
-      <c r="F59" t="s">
-        <v>22</v>
+      <c r="F59" t="n">
+        <v>0</v>
       </c>
       <c r="G59" t="n">
         <v>1</v>
@@ -4746,7 +4744,7 @@
     </row>
     <row r="60" spans="1:22">
       <c r="A60" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B60" t="n">
         <v>4.38942</v>
@@ -4760,8 +4758,8 @@
       <c r="E60" t="n">
         <v>14</v>
       </c>
-      <c r="F60" t="s">
-        <v>22</v>
+      <c r="F60" t="n">
+        <v>0</v>
       </c>
       <c r="G60" t="n">
         <v>1</v>
@@ -4814,7 +4812,7 @@
     </row>
     <row r="61" spans="1:22">
       <c r="A61" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B61" t="n">
         <v>6.81796</v>
@@ -4828,8 +4826,8 @@
       <c r="E61" t="n">
         <v>2</v>
       </c>
-      <c r="F61" t="s">
-        <v>22</v>
+      <c r="F61" t="n">
+        <v>0</v>
       </c>
       <c r="G61" t="n">
         <v>1</v>
@@ -4882,7 +4880,7 @@
     </row>
     <row r="62" spans="1:22">
       <c r="A62" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B62" t="n">
         <v>4.73348</v>
@@ -4896,8 +4894,8 @@
       <c r="E62" t="n">
         <v>0</v>
       </c>
-      <c r="F62" t="s">
-        <v>22</v>
+      <c r="F62" t="n">
+        <v>0</v>
       </c>
       <c r="G62" t="n">
         <v>1</v>
@@ -4950,7 +4948,7 @@
     </row>
     <row r="63" spans="1:22">
       <c r="A63" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B63" t="n">
         <v>8.93329</v>
@@ -4964,8 +4962,8 @@
       <c r="E63" t="n">
         <v>0</v>
       </c>
-      <c r="F63" t="s">
-        <v>22</v>
+      <c r="F63" t="n">
+        <v>0</v>
       </c>
       <c r="G63" t="n">
         <v>1</v>
@@ -5018,7 +5016,7 @@
     </row>
     <row r="64" spans="1:22">
       <c r="A64" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B64" t="n">
         <v>5.83584</v>
@@ -5032,8 +5030,8 @@
       <c r="E64" t="n">
         <v>0</v>
       </c>
-      <c r="F64" t="s">
-        <v>22</v>
+      <c r="F64" t="n">
+        <v>0</v>
       </c>
       <c r="G64" t="n">
         <v>1</v>
@@ -5086,7 +5084,7 @@
     </row>
     <row r="65" spans="1:22">
       <c r="A65" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B65" t="n">
         <v>7.18498</v>
@@ -5100,8 +5098,8 @@
       <c r="E65" t="n">
         <v>14</v>
       </c>
-      <c r="F65" t="s">
-        <v>22</v>
+      <c r="F65" t="n">
+        <v>0</v>
       </c>
       <c r="G65" t="n">
         <v>1</v>
@@ -5154,7 +5152,7 @@
     </row>
     <row r="66" spans="1:22">
       <c r="A66" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B66" t="n">
         <v>5.92242</v>
@@ -5168,8 +5166,8 @@
       <c r="E66" t="n">
         <v>0</v>
       </c>
-      <c r="F66" t="s">
-        <v>22</v>
+      <c r="F66" t="n">
+        <v>0</v>
       </c>
       <c r="G66" t="n">
         <v>1</v>
@@ -5222,7 +5220,7 @@
     </row>
     <row r="67" spans="1:22">
       <c r="A67" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B67" t="n">
         <v>9.2446</v>
@@ -5236,8 +5234,8 @@
       <c r="E67" t="n">
         <v>23</v>
       </c>
-      <c r="F67" t="s">
-        <v>22</v>
+      <c r="F67" t="n">
+        <v>0</v>
       </c>
       <c r="G67" t="n">
         <v>1</v>
@@ -5290,7 +5288,7 @@
     </row>
     <row r="68" spans="1:22">
       <c r="A68" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B68" t="n">
         <v>5.50827</v>
@@ -5304,8 +5302,8 @@
       <c r="E68" t="n">
         <v>3</v>
       </c>
-      <c r="F68" t="s">
-        <v>22</v>
+      <c r="F68" t="n">
+        <v>0</v>
       </c>
       <c r="G68" t="n">
         <v>1</v>
@@ -5358,7 +5356,7 @@
     </row>
     <row r="69" spans="1:22">
       <c r="A69" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B69" t="n">
         <v>4.82089</v>
@@ -5372,8 +5370,8 @@
       <c r="E69" t="n">
         <v>24</v>
       </c>
-      <c r="F69" t="s">
-        <v>22</v>
+      <c r="F69" t="n">
+        <v>0</v>
       </c>
       <c r="G69" t="n">
         <v>1</v>
@@ -5426,7 +5424,7 @@
     </row>
     <row r="70" spans="1:22">
       <c r="A70" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B70" t="n">
         <v>5.28947</v>
@@ -5440,8 +5438,8 @@
       <c r="E70" t="n">
         <v>3</v>
       </c>
-      <c r="F70" t="s">
-        <v>22</v>
+      <c r="F70" t="n">
+        <v>0</v>
       </c>
       <c r="G70" t="n">
         <v>1</v>
@@ -5494,7 +5492,7 @@
     </row>
     <row r="71" spans="1:22">
       <c r="A71" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B71" t="n">
         <v>7.82746</v>
@@ -5508,8 +5506,8 @@
       <c r="E71" t="n">
         <v>5</v>
       </c>
-      <c r="F71" t="s">
-        <v>22</v>
+      <c r="F71" t="n">
+        <v>0</v>
       </c>
       <c r="G71" t="n">
         <v>1</v>
@@ -5562,7 +5560,7 @@
     </row>
     <row r="72" spans="1:22">
       <c r="A72" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B72" t="n">
         <v>4.9001</v>
@@ -5576,8 +5574,8 @@
       <c r="E72" t="n">
         <v>3</v>
       </c>
-      <c r="F72" t="s">
-        <v>22</v>
+      <c r="F72" t="n">
+        <v>0</v>
       </c>
       <c r="G72" t="n">
         <v>1</v>
@@ -5630,7 +5628,7 @@
     </row>
     <row r="73" spans="1:22">
       <c r="A73" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B73" t="n">
         <v>4.30566</v>
@@ -5644,8 +5642,8 @@
       <c r="E73" t="n">
         <v>3</v>
       </c>
-      <c r="F73" t="s">
-        <v>22</v>
+      <c r="F73" t="n">
+        <v>0</v>
       </c>
       <c r="G73" t="n">
         <v>1</v>
@@ -5698,7 +5696,7 @@
     </row>
     <row r="74" spans="1:22">
       <c r="A74" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B74" t="n">
         <v>5.72296</v>
@@ -5712,8 +5710,8 @@
       <c r="E74" t="n">
         <v>8</v>
       </c>
-      <c r="F74" t="s">
-        <v>22</v>
+      <c r="F74" t="n">
+        <v>0</v>
       </c>
       <c r="G74" t="n">
         <v>1</v>
@@ -5766,20 +5764,22 @@
     </row>
     <row r="75" spans="1:22">
       <c r="A75" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B75" t="n">
         <v>5.12452</v>
       </c>
-      <c r="C75" t="s"/>
+      <c r="C75" t="n">
+        <v>2015</v>
+      </c>
       <c r="D75" t="n">
         <v>7</v>
       </c>
       <c r="E75" t="n">
         <v>15</v>
       </c>
-      <c r="F75" t="s">
-        <v>22</v>
+      <c r="F75" t="n">
+        <v>0</v>
       </c>
       <c r="G75" t="n">
         <v>1</v>
@@ -5832,20 +5832,22 @@
     </row>
     <row r="76" spans="1:22">
       <c r="A76" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B76" t="n">
         <v>9.167149999999999</v>
       </c>
-      <c r="C76" t="s"/>
+      <c r="C76" t="n">
+        <v>2015</v>
+      </c>
       <c r="D76" t="n">
         <v>298</v>
       </c>
       <c r="E76" t="n">
         <v>1</v>
       </c>
-      <c r="F76" t="s">
-        <v>22</v>
+      <c r="F76" t="n">
+        <v>0</v>
       </c>
       <c r="G76" t="n">
         <v>1</v>
@@ -5898,7 +5900,7 @@
     </row>
     <row r="77" spans="1:22">
       <c r="A77" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B77" t="n">
         <v>8.41846</v>
@@ -5912,8 +5914,8 @@
       <c r="E77" t="n">
         <v>25</v>
       </c>
-      <c r="F77" t="s">
-        <v>22</v>
+      <c r="F77" t="n">
+        <v>0</v>
       </c>
       <c r="G77" t="n">
         <v>1</v>
@@ -5966,7 +5968,7 @@
     </row>
     <row r="78" spans="1:22">
       <c r="A78" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B78" t="n">
         <v>6.55822</v>
@@ -5980,8 +5982,8 @@
       <c r="E78" t="n">
         <v>2</v>
       </c>
-      <c r="F78" t="s">
-        <v>22</v>
+      <c r="F78" t="n">
+        <v>0</v>
       </c>
       <c r="G78" t="n">
         <v>1</v>
@@ -6034,7 +6036,7 @@
     </row>
     <row r="79" spans="1:22">
       <c r="A79" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B79" t="n">
         <v>7.42313</v>
@@ -6048,8 +6050,8 @@
       <c r="E79" t="n">
         <v>10</v>
       </c>
-      <c r="F79" t="s">
-        <v>22</v>
+      <c r="F79" t="n">
+        <v>0</v>
       </c>
       <c r="G79" t="n">
         <v>1</v>
@@ -6102,7 +6104,7 @@
     </row>
     <row r="80" spans="1:22">
       <c r="A80" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B80" t="n">
         <v>7.34378</v>
@@ -6116,8 +6118,8 @@
       <c r="E80" t="n">
         <v>10</v>
       </c>
-      <c r="F80" t="s">
-        <v>22</v>
+      <c r="F80" t="n">
+        <v>0</v>
       </c>
       <c r="G80" t="n">
         <v>1</v>
@@ -6170,7 +6172,7 @@
     </row>
     <row r="81" spans="1:22">
       <c r="A81" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B81" t="n">
         <v>5.16565</v>
@@ -6184,8 +6186,8 @@
       <c r="E81" t="n">
         <v>0</v>
       </c>
-      <c r="F81" t="s">
-        <v>22</v>
+      <c r="F81" t="n">
+        <v>0</v>
       </c>
       <c r="G81" t="n">
         <v>1</v>
@@ -6238,20 +6240,22 @@
     </row>
     <row r="82" spans="1:22">
       <c r="A82" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B82" t="n">
         <v>7.87298</v>
       </c>
-      <c r="C82" t="s"/>
+      <c r="C82" t="n">
+        <v>2015</v>
+      </c>
       <c r="D82" t="n">
         <v>35</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
       </c>
-      <c r="F82" t="s">
-        <v>22</v>
+      <c r="F82" t="n">
+        <v>0</v>
       </c>
       <c r="G82" t="n">
         <v>1</v>
@@ -6304,7 +6308,7 @@
     </row>
     <row r="83" spans="1:22">
       <c r="A83" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B83" t="n">
         <v>5.10454</v>
@@ -6318,8 +6322,8 @@
       <c r="E83" t="n">
         <v>2</v>
       </c>
-      <c r="F83" t="s">
-        <v>22</v>
+      <c r="F83" t="n">
+        <v>0</v>
       </c>
       <c r="G83" t="n">
         <v>1</v>
@@ -6372,7 +6376,7 @@
     </row>
     <row r="84" spans="1:22">
       <c r="A84" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B84" t="n">
         <v>7.13238</v>
@@ -6386,8 +6390,8 @@
       <c r="E84" t="n">
         <v>12</v>
       </c>
-      <c r="F84" t="s">
-        <v>22</v>
+      <c r="F84" t="n">
+        <v>0</v>
       </c>
       <c r="G84" t="n">
         <v>1</v>
@@ -6440,7 +6444,7 @@
     </row>
     <row r="85" spans="1:22">
       <c r="A85" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B85" t="n">
         <v>8.62795</v>
@@ -6454,8 +6458,8 @@
       <c r="E85" t="n">
         <v>5</v>
       </c>
-      <c r="F85" t="s">
-        <v>22</v>
+      <c r="F85" t="n">
+        <v>0</v>
       </c>
       <c r="G85" t="n">
         <v>1</v>
@@ -6508,7 +6512,7 @@
     </row>
     <row r="86" spans="1:22">
       <c r="A86" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B86" t="n">
         <v>7.58363</v>
@@ -6522,8 +6526,8 @@
       <c r="E86" t="n">
         <v>15</v>
       </c>
-      <c r="F86" t="s">
-        <v>22</v>
+      <c r="F86" t="n">
+        <v>0</v>
       </c>
       <c r="G86" t="n">
         <v>1</v>
@@ -6576,7 +6580,7 @@
     </row>
     <row r="87" spans="1:22">
       <c r="A87" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B87" t="n">
         <v>6.53666</v>
@@ -6590,8 +6594,8 @@
       <c r="E87" t="n">
         <v>3</v>
       </c>
-      <c r="F87" t="s">
-        <v>22</v>
+      <c r="F87" t="n">
+        <v>0</v>
       </c>
       <c r="G87" t="n">
         <v>1</v>
@@ -6644,7 +6648,7 @@
     </row>
     <row r="88" spans="1:22">
       <c r="A88" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B88" t="n">
         <v>3.84745</v>
@@ -6658,8 +6662,8 @@
       <c r="E88" t="n">
         <v>0</v>
       </c>
-      <c r="F88" t="s">
-        <v>22</v>
+      <c r="F88" t="n">
+        <v>0</v>
       </c>
       <c r="G88" t="n">
         <v>1</v>
@@ -6712,7 +6716,7 @@
     </row>
     <row r="89" spans="1:22">
       <c r="A89" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B89" t="n">
         <v>4.38168</v>
@@ -6726,8 +6730,8 @@
       <c r="E89" t="n">
         <v>1</v>
       </c>
-      <c r="F89" t="s">
-        <v>22</v>
+      <c r="F89" t="n">
+        <v>0</v>
       </c>
       <c r="G89" t="n">
         <v>1</v>
@@ -6780,20 +6784,22 @@
     </row>
     <row r="90" spans="1:22">
       <c r="A90" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B90" t="n">
         <v>7.85074</v>
       </c>
-      <c r="C90" t="s"/>
+      <c r="C90" t="n">
+        <v>2015</v>
+      </c>
       <c r="D90" t="n">
         <v>23</v>
       </c>
       <c r="E90" t="n">
         <v>2</v>
       </c>
-      <c r="F90" t="s">
-        <v>22</v>
+      <c r="F90" t="n">
+        <v>0</v>
       </c>
       <c r="G90" t="n">
         <v>1</v>
@@ -6846,7 +6852,7 @@
     </row>
     <row r="91" spans="1:22">
       <c r="A91" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B91" t="n">
         <v>7.51725</v>
@@ -6860,8 +6866,8 @@
       <c r="E91" t="n">
         <v>4</v>
       </c>
-      <c r="F91" t="s">
-        <v>22</v>
+      <c r="F91" t="n">
+        <v>0</v>
       </c>
       <c r="G91" t="n">
         <v>1</v>
@@ -6914,7 +6920,7 @@
     </row>
     <row r="92" spans="1:22">
       <c r="A92" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B92" t="n">
         <v>8.411849999999999</v>
@@ -6928,8 +6934,8 @@
       <c r="E92" t="n">
         <v>1</v>
       </c>
-      <c r="F92" t="s">
-        <v>22</v>
+      <c r="F92" t="n">
+        <v>0</v>
       </c>
       <c r="G92" t="n">
         <v>1</v>
@@ -6982,7 +6988,7 @@
     </row>
     <row r="93" spans="1:22">
       <c r="A93" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B93" t="n">
         <v>9.432359999999999</v>
@@ -6996,8 +7002,8 @@
       <c r="E93" t="n">
         <v>1</v>
       </c>
-      <c r="F93" t="s">
-        <v>22</v>
+      <c r="F93" t="n">
+        <v>0</v>
       </c>
       <c r="G93" t="n">
         <v>1</v>
@@ -7050,7 +7056,7 @@
     </row>
     <row r="94" spans="1:22">
       <c r="A94" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B94" t="n">
         <v>3.82664</v>
@@ -7064,8 +7070,8 @@
       <c r="E94" t="n">
         <v>49</v>
       </c>
-      <c r="F94" t="s">
-        <v>22</v>
+      <c r="F94" t="n">
+        <v>0</v>
       </c>
       <c r="G94" t="n">
         <v>1</v>
@@ -7118,20 +7124,22 @@
     </row>
     <row r="95" spans="1:22">
       <c r="A95" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B95" t="n">
         <v>7.81916</v>
       </c>
-      <c r="C95" t="s"/>
+      <c r="C95" t="n">
+        <v>2015</v>
+      </c>
       <c r="D95" t="n">
         <v>51</v>
       </c>
       <c r="E95" t="n">
         <v>3</v>
       </c>
-      <c r="F95" t="s">
-        <v>22</v>
+      <c r="F95" t="n">
+        <v>0</v>
       </c>
       <c r="G95" t="n">
         <v>1</v>
@@ -7184,7 +7192,7 @@
     </row>
     <row r="96" spans="1:22">
       <c r="A96" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B96" t="n">
         <v>5.21645</v>
@@ -7198,8 +7206,8 @@
       <c r="E96" t="n">
         <v>2</v>
       </c>
-      <c r="F96" t="s">
-        <v>22</v>
+      <c r="F96" t="n">
+        <v>0</v>
       </c>
       <c r="G96" t="n">
         <v>1</v>
@@ -7252,7 +7260,7 @@
     </row>
     <row r="97" spans="1:22">
       <c r="A97" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B97" t="n">
         <v>3.83104</v>
@@ -7266,8 +7274,8 @@
       <c r="E97" t="n">
         <v>19</v>
       </c>
-      <c r="F97" t="s">
-        <v>22</v>
+      <c r="F97" t="n">
+        <v>0</v>
       </c>
       <c r="G97" t="n">
         <v>1</v>
@@ -7320,7 +7328,7 @@
     </row>
     <row r="98" spans="1:22">
       <c r="A98" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B98" t="n">
         <v>5.03235</v>
@@ -7334,8 +7342,8 @@
       <c r="E98" t="n">
         <v>2</v>
       </c>
-      <c r="F98" t="s">
-        <v>22</v>
+      <c r="F98" t="n">
+        <v>0</v>
       </c>
       <c r="G98" t="n">
         <v>1</v>
@@ -7388,7 +7396,7 @@
     </row>
     <row r="99" spans="1:22">
       <c r="A99" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B99" t="n">
         <v>5.24821</v>
@@ -7402,8 +7410,8 @@
       <c r="E99" t="n">
         <v>5</v>
       </c>
-      <c r="F99" t="s">
-        <v>22</v>
+      <c r="F99" t="n">
+        <v>0</v>
       </c>
       <c r="G99" t="n">
         <v>1</v>
@@ -7456,7 +7464,7 @@
     </row>
     <row r="100" spans="1:22">
       <c r="A100" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B100" t="n">
         <v>6.19419</v>
@@ -7470,8 +7478,8 @@
       <c r="E100" t="n">
         <v>1</v>
       </c>
-      <c r="F100" t="s">
-        <v>22</v>
+      <c r="F100" t="n">
+        <v>0</v>
       </c>
       <c r="G100" t="n">
         <v>1</v>
@@ -7524,7 +7532,7 @@
     </row>
     <row r="101" spans="1:22">
       <c r="A101" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B101" t="n">
         <v>5.03984</v>
@@ -7538,8 +7546,8 @@
       <c r="E101" t="n">
         <v>1</v>
       </c>
-      <c r="F101" t="s">
-        <v>22</v>
+      <c r="F101" t="n">
+        <v>0</v>
       </c>
       <c r="G101" t="n">
         <v>1</v>

</xml_diff>